<commit_message>
add time test data
</commit_message>
<xml_diff>
--- a/论文/TimeTest.xlsx
+++ b/论文/TimeTest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UppreSSO-Code-Flow-main\论文\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F167D14D-7CE3-49D3-837B-FCDDDBFAE010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2CBABA3-2BC2-4DDB-AE37-425FF64C7A02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5040" yWindow="864" windowWidth="23040" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="11">
   <si>
     <t>MITREDID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -76,6 +76,10 @@
   </si>
   <si>
     <t>UPPRESSO_RING_MODE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UPPRESSO_PPTOKEN_MODE</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -407,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O13"/>
+  <dimension ref="A1:W13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="T20" sqref="T20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -426,14 +430,20 @@
     <col min="12" max="12" width="14.77734375" customWidth="1"/>
     <col min="13" max="13" width="12.88671875" customWidth="1"/>
     <col min="14" max="14" width="10.33203125" customWidth="1"/>
+    <col min="17" max="17" width="25.88671875" customWidth="1"/>
+    <col min="18" max="18" width="16.44140625" customWidth="1"/>
+    <col min="19" max="19" width="11.5546875" customWidth="1"/>
+    <col min="20" max="20" width="14.5546875" customWidth="1"/>
+    <col min="21" max="21" width="12.88671875" customWidth="1"/>
+    <col min="22" max="22" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -476,8 +486,29 @@
       <c r="O2" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="Q2" t="s">
+        <v>10</v>
+      </c>
+      <c r="R2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S2" t="s">
+        <v>1</v>
+      </c>
+      <c r="T2" t="s">
+        <v>3</v>
+      </c>
+      <c r="U2" t="s">
+        <v>4</v>
+      </c>
+      <c r="V2" t="s">
+        <v>5</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -520,8 +551,29 @@
       <c r="O3" s="2">
         <v>0</v>
       </c>
+      <c r="Q3" s="2">
+        <v>1</v>
+      </c>
+      <c r="R3" s="2">
+        <v>808</v>
+      </c>
+      <c r="S3" s="2">
+        <v>18</v>
+      </c>
+      <c r="T3" s="2">
+        <v>1020</v>
+      </c>
+      <c r="U3" s="2">
+        <v>378</v>
+      </c>
+      <c r="V3" s="2">
+        <v>6005</v>
+      </c>
+      <c r="W3" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -564,8 +616,29 @@
       <c r="O4" s="2">
         <v>0</v>
       </c>
+      <c r="Q4" s="2">
+        <v>2</v>
+      </c>
+      <c r="R4" s="2">
+        <v>808</v>
+      </c>
+      <c r="S4" s="2">
+        <v>19</v>
+      </c>
+      <c r="T4" s="2">
+        <v>1114</v>
+      </c>
+      <c r="U4" s="2">
+        <v>372</v>
+      </c>
+      <c r="V4" s="2">
+        <v>6255</v>
+      </c>
+      <c r="W4" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -608,8 +681,29 @@
       <c r="O5" s="2">
         <v>0</v>
       </c>
+      <c r="Q5" s="2">
+        <v>3</v>
+      </c>
+      <c r="R5" s="2">
+        <v>786</v>
+      </c>
+      <c r="S5" s="2">
+        <v>23</v>
+      </c>
+      <c r="T5" s="2">
+        <v>1171</v>
+      </c>
+      <c r="U5" s="2">
+        <v>407</v>
+      </c>
+      <c r="V5" s="2">
+        <v>5934</v>
+      </c>
+      <c r="W5" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -652,8 +746,29 @@
       <c r="O6" s="2">
         <v>0</v>
       </c>
+      <c r="Q6" s="2">
+        <v>4</v>
+      </c>
+      <c r="R6" s="2">
+        <v>802</v>
+      </c>
+      <c r="S6" s="2">
+        <v>23</v>
+      </c>
+      <c r="T6" s="2">
+        <v>1171</v>
+      </c>
+      <c r="U6" s="2">
+        <v>358</v>
+      </c>
+      <c r="V6" s="2">
+        <v>6063</v>
+      </c>
+      <c r="W6" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -696,8 +811,29 @@
       <c r="O7" s="2">
         <v>0</v>
       </c>
+      <c r="Q7" s="2">
+        <v>5</v>
+      </c>
+      <c r="R7" s="2">
+        <v>879</v>
+      </c>
+      <c r="S7" s="2">
+        <v>19</v>
+      </c>
+      <c r="T7" s="2">
+        <v>1231</v>
+      </c>
+      <c r="U7" s="2">
+        <v>363</v>
+      </c>
+      <c r="V7" s="2">
+        <v>6412</v>
+      </c>
+      <c r="W7" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -740,8 +876,29 @@
       <c r="O8" s="2">
         <v>0</v>
       </c>
+      <c r="Q8" s="2">
+        <v>6</v>
+      </c>
+      <c r="R8" s="2">
+        <v>791</v>
+      </c>
+      <c r="S8" s="2">
+        <v>25</v>
+      </c>
+      <c r="T8" s="2">
+        <v>965</v>
+      </c>
+      <c r="U8" s="2">
+        <v>372</v>
+      </c>
+      <c r="V8" s="2">
+        <v>5581</v>
+      </c>
+      <c r="W8" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -784,8 +941,29 @@
       <c r="O9" s="2">
         <v>0</v>
       </c>
+      <c r="Q9" s="2">
+        <v>7</v>
+      </c>
+      <c r="R9" s="2">
+        <v>874</v>
+      </c>
+      <c r="S9" s="2">
+        <v>19</v>
+      </c>
+      <c r="T9" s="2">
+        <v>1196</v>
+      </c>
+      <c r="U9" s="2">
+        <v>382</v>
+      </c>
+      <c r="V9" s="2">
+        <v>6168</v>
+      </c>
+      <c r="W9" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -828,8 +1006,29 @@
       <c r="O10" s="2">
         <v>0</v>
       </c>
+      <c r="Q10" s="2">
+        <v>8</v>
+      </c>
+      <c r="R10" s="2">
+        <v>736</v>
+      </c>
+      <c r="S10" s="2">
+        <v>21</v>
+      </c>
+      <c r="T10" s="2">
+        <v>1244</v>
+      </c>
+      <c r="U10" s="2">
+        <v>375</v>
+      </c>
+      <c r="V10" s="2">
+        <v>6245</v>
+      </c>
+      <c r="W10" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -872,8 +1071,29 @@
       <c r="O11" s="2">
         <v>0</v>
       </c>
+      <c r="Q11" s="2">
+        <v>9</v>
+      </c>
+      <c r="R11" s="2">
+        <v>813</v>
+      </c>
+      <c r="S11" s="2">
+        <v>20</v>
+      </c>
+      <c r="T11" s="2">
+        <v>1079</v>
+      </c>
+      <c r="U11" s="2">
+        <v>405</v>
+      </c>
+      <c r="V11" s="2">
+        <v>6011</v>
+      </c>
+      <c r="W11" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -916,8 +1136,29 @@
       <c r="O12" s="2">
         <v>0</v>
       </c>
+      <c r="Q12" s="2">
+        <v>10</v>
+      </c>
+      <c r="R12" s="2">
+        <v>937</v>
+      </c>
+      <c r="S12" s="2">
+        <v>22</v>
+      </c>
+      <c r="T12" s="2">
+        <v>1030</v>
+      </c>
+      <c r="U12" s="2">
+        <v>378</v>
+      </c>
+      <c r="V12" s="2">
+        <v>6249</v>
+      </c>
+      <c r="W12" s="2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
@@ -968,6 +1209,32 @@
         <v>6120.9</v>
       </c>
       <c r="O13" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="R13" s="2">
+        <f>AVERAGE(R3:R12)</f>
+        <v>823.4</v>
+      </c>
+      <c r="S13" s="2">
+        <f>AVERAGE(S3:S12)</f>
+        <v>20.9</v>
+      </c>
+      <c r="T13" s="2">
+        <f>AVERAGE(T3:T12)</f>
+        <v>1122.0999999999999</v>
+      </c>
+      <c r="U13" s="2">
+        <f>AVERAGE(U3:U12)</f>
+        <v>379</v>
+      </c>
+      <c r="V13" s="2">
+        <f>AVERAGE(V3:V12)</f>
+        <v>6092.3</v>
+      </c>
+      <c r="W13" s="2">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Time test data  finished.
</commit_message>
<xml_diff>
--- a/论文/TimeTest.xlsx
+++ b/论文/TimeTest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UppreSSO-Code-Flow-main\论文\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2CBABA3-2BC2-4DDB-AE37-425FF64C7A02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC21E163-1BFC-414B-A294-41512AB94F0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5040" yWindow="864" windowWidth="23040" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="20">
   <si>
     <t>MITREDID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -63,10 +63,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>rtt</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>单位:ms</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -80,6 +76,44 @@
   </si>
   <si>
     <t>UPPRESSO_PPTOKEN_MODE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rtt/bandwidth</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0/Unlimited</t>
+  </si>
+  <si>
+    <t>0/Unlimited</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>96/100Mbps</t>
+  </si>
+  <si>
+    <t>96/100Mbps</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SSO System</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RTT/Bandwidth</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UPPRESSO_RING</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UPRRESSO_PPTOKEN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Total</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -123,10 +157,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -411,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W13"/>
+  <dimension ref="A1:W38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="T20" sqref="T20"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O36" sqref="O36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -423,24 +460,27 @@
     <col min="3" max="3" width="11.44140625" customWidth="1"/>
     <col min="4" max="4" width="14.77734375" customWidth="1"/>
     <col min="5" max="5" width="13.109375" customWidth="1"/>
-    <col min="6" max="7" width="10.6640625" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" customWidth="1"/>
     <col min="9" max="9" width="22.21875" customWidth="1"/>
     <col min="10" max="10" width="16.5546875" customWidth="1"/>
-    <col min="11" max="11" width="11.88671875" customWidth="1"/>
-    <col min="12" max="12" width="14.77734375" customWidth="1"/>
-    <col min="13" max="13" width="12.88671875" customWidth="1"/>
-    <col min="14" max="14" width="10.33203125" customWidth="1"/>
+    <col min="11" max="11" width="18.33203125" customWidth="1"/>
+    <col min="12" max="12" width="16.88671875" customWidth="1"/>
+    <col min="13" max="13" width="13.88671875" customWidth="1"/>
+    <col min="14" max="14" width="13.33203125" customWidth="1"/>
+    <col min="15" max="15" width="14.88671875" customWidth="1"/>
     <col min="17" max="17" width="25.88671875" customWidth="1"/>
     <col min="18" max="18" width="16.44140625" customWidth="1"/>
     <col min="19" max="19" width="11.5546875" customWidth="1"/>
     <col min="20" max="20" width="14.5546875" customWidth="1"/>
     <col min="21" max="21" width="12.88671875" customWidth="1"/>
     <col min="22" max="22" width="10.6640625" customWidth="1"/>
+    <col min="23" max="23" width="15.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
@@ -463,31 +503,31 @@
         <v>5</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q2" t="s">
         <v>9</v>
-      </c>
-      <c r="J2" t="s">
-        <v>2</v>
-      </c>
-      <c r="K2" t="s">
-        <v>1</v>
-      </c>
-      <c r="L2" t="s">
-        <v>3</v>
-      </c>
-      <c r="M2" t="s">
-        <v>4</v>
-      </c>
-      <c r="N2" t="s">
-        <v>5</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>10</v>
       </c>
       <c r="R2" t="s">
         <v>2</v>
@@ -505,7 +545,7 @@
         <v>5</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
@@ -527,8 +567,8 @@
       <c r="F3" s="2">
         <v>7151</v>
       </c>
-      <c r="G3" s="2">
-        <v>0</v>
+      <c r="G3" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="I3" s="2">
         <v>1</v>
@@ -548,8 +588,8 @@
       <c r="N3" s="2">
         <v>6094</v>
       </c>
-      <c r="O3" s="2">
-        <v>0</v>
+      <c r="O3" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="Q3" s="2">
         <v>1</v>
@@ -569,8 +609,8 @@
       <c r="V3" s="2">
         <v>6005</v>
       </c>
-      <c r="W3" s="2">
-        <v>0</v>
+      <c r="W3" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
@@ -592,8 +632,8 @@
       <c r="F4" s="2">
         <v>6103</v>
       </c>
-      <c r="G4" s="2">
-        <v>0</v>
+      <c r="G4" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="I4" s="2">
         <v>2</v>
@@ -613,8 +653,8 @@
       <c r="N4" s="2">
         <v>5896</v>
       </c>
-      <c r="O4" s="2">
-        <v>0</v>
+      <c r="O4" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="Q4" s="2">
         <v>2</v>
@@ -634,8 +674,8 @@
       <c r="V4" s="2">
         <v>6255</v>
       </c>
-      <c r="W4" s="2">
-        <v>0</v>
+      <c r="W4" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
@@ -657,8 +697,8 @@
       <c r="F5" s="2">
         <v>6499</v>
       </c>
-      <c r="G5" s="2">
-        <v>0</v>
+      <c r="G5" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="I5" s="2">
         <v>3</v>
@@ -678,8 +718,8 @@
       <c r="N5" s="2">
         <v>6636</v>
       </c>
-      <c r="O5" s="2">
-        <v>0</v>
+      <c r="O5" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="Q5" s="2">
         <v>3</v>
@@ -699,8 +739,8 @@
       <c r="V5" s="2">
         <v>5934</v>
       </c>
-      <c r="W5" s="2">
-        <v>0</v>
+      <c r="W5" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
@@ -722,8 +762,8 @@
       <c r="F6" s="2">
         <v>6086</v>
       </c>
-      <c r="G6" s="2">
-        <v>0</v>
+      <c r="G6" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="I6" s="2">
         <v>4</v>
@@ -743,8 +783,8 @@
       <c r="N6" s="2">
         <v>5906</v>
       </c>
-      <c r="O6" s="2">
-        <v>0</v>
+      <c r="O6" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="Q6" s="2">
         <v>4</v>
@@ -764,8 +804,8 @@
       <c r="V6" s="2">
         <v>6063</v>
       </c>
-      <c r="W6" s="2">
-        <v>0</v>
+      <c r="W6" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
@@ -787,8 +827,8 @@
       <c r="F7" s="2">
         <v>6913</v>
       </c>
-      <c r="G7" s="2">
-        <v>0</v>
+      <c r="G7" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="I7" s="2">
         <v>5</v>
@@ -808,8 +848,8 @@
       <c r="N7" s="2">
         <v>6064</v>
       </c>
-      <c r="O7" s="2">
-        <v>0</v>
+      <c r="O7" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="Q7" s="2">
         <v>5</v>
@@ -829,8 +869,8 @@
       <c r="V7" s="2">
         <v>6412</v>
       </c>
-      <c r="W7" s="2">
-        <v>0</v>
+      <c r="W7" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
@@ -852,8 +892,8 @@
       <c r="F8" s="2">
         <v>6653</v>
       </c>
-      <c r="G8" s="2">
-        <v>0</v>
+      <c r="G8" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="I8" s="2">
         <v>6</v>
@@ -873,8 +913,8 @@
       <c r="N8" s="2">
         <v>6197</v>
       </c>
-      <c r="O8" s="2">
-        <v>0</v>
+      <c r="O8" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="Q8" s="2">
         <v>6</v>
@@ -894,8 +934,8 @@
       <c r="V8" s="2">
         <v>5581</v>
       </c>
-      <c r="W8" s="2">
-        <v>0</v>
+      <c r="W8" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
@@ -917,8 +957,8 @@
       <c r="F9" s="2">
         <v>6558</v>
       </c>
-      <c r="G9" s="2">
-        <v>0</v>
+      <c r="G9" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="I9" s="2">
         <v>7</v>
@@ -938,8 +978,8 @@
       <c r="N9" s="2">
         <v>6279</v>
       </c>
-      <c r="O9" s="2">
-        <v>0</v>
+      <c r="O9" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="Q9" s="2">
         <v>7</v>
@@ -959,8 +999,8 @@
       <c r="V9" s="2">
         <v>6168</v>
       </c>
-      <c r="W9" s="2">
-        <v>0</v>
+      <c r="W9" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
@@ -982,8 +1022,8 @@
       <c r="F10" s="2">
         <v>6948</v>
       </c>
-      <c r="G10" s="2">
-        <v>0</v>
+      <c r="G10" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="I10" s="2">
         <v>8</v>
@@ -1003,8 +1043,8 @@
       <c r="N10" s="2">
         <v>5975</v>
       </c>
-      <c r="O10" s="2">
-        <v>0</v>
+      <c r="O10" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="Q10" s="2">
         <v>8</v>
@@ -1024,8 +1064,8 @@
       <c r="V10" s="2">
         <v>6245</v>
       </c>
-      <c r="W10" s="2">
-        <v>0</v>
+      <c r="W10" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
@@ -1047,8 +1087,8 @@
       <c r="F11" s="2">
         <v>6610</v>
       </c>
-      <c r="G11" s="2">
-        <v>0</v>
+      <c r="G11" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="I11" s="2">
         <v>9</v>
@@ -1068,8 +1108,8 @@
       <c r="N11" s="2">
         <v>6027</v>
       </c>
-      <c r="O11" s="2">
-        <v>0</v>
+      <c r="O11" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="Q11" s="2">
         <v>9</v>
@@ -1089,8 +1129,8 @@
       <c r="V11" s="2">
         <v>6011</v>
       </c>
-      <c r="W11" s="2">
-        <v>0</v>
+      <c r="W11" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
@@ -1112,8 +1152,8 @@
       <c r="F12" s="1">
         <v>6512</v>
       </c>
-      <c r="G12" s="2">
-        <v>0</v>
+      <c r="G12" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="I12" s="2">
         <v>10</v>
@@ -1133,8 +1173,8 @@
       <c r="N12" s="2">
         <v>6135</v>
       </c>
-      <c r="O12" s="2">
-        <v>0</v>
+      <c r="O12" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="Q12" s="2">
         <v>10</v>
@@ -1154,13 +1194,13 @@
       <c r="V12" s="2">
         <v>6249</v>
       </c>
-      <c r="W12" s="2">
-        <v>0</v>
+      <c r="W12" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B13" s="1">
         <f>AVERAGE(B3:B12)</f>
@@ -1182,11 +1222,11 @@
         <f>AVERAGE(F3:F12)</f>
         <v>6603.3</v>
       </c>
-      <c r="G13" s="1">
-        <v>0</v>
+      <c r="G13" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J13" s="2">
         <f>AVERAGE(J3:J12)</f>
@@ -1208,11 +1248,11 @@
         <f>AVERAGE(N3:N12)</f>
         <v>6120.9</v>
       </c>
-      <c r="O13" s="2">
-        <v>0</v>
+      <c r="O13" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="R13" s="2">
         <f>AVERAGE(R3:R12)</f>
@@ -1234,11 +1274,1012 @@
         <f>AVERAGE(V3:V12)</f>
         <v>6092.3</v>
       </c>
-      <c r="W13" s="2">
+      <c r="W13" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="B16" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="N16" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="O16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>9</v>
+      </c>
+      <c r="R16" t="s">
+        <v>2</v>
+      </c>
+      <c r="S16" t="s">
+        <v>1</v>
+      </c>
+      <c r="T16" t="s">
+        <v>3</v>
+      </c>
+      <c r="U16" t="s">
+        <v>4</v>
+      </c>
+      <c r="V16" t="s">
+        <v>5</v>
+      </c>
+      <c r="W16" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>1</v>
+      </c>
+      <c r="B17" s="2">
+        <v>999</v>
+      </c>
+      <c r="C17" s="2">
+        <v>741</v>
+      </c>
+      <c r="D17" s="2">
+        <v>2567</v>
+      </c>
+      <c r="E17" s="2">
+        <v>288</v>
+      </c>
+      <c r="F17" s="2">
+        <v>10587</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I17" s="2">
+        <v>1</v>
+      </c>
+      <c r="J17" s="2">
+        <v>1901</v>
+      </c>
+      <c r="K17" s="2">
+        <v>38</v>
+      </c>
+      <c r="L17" s="2">
+        <v>2898</v>
+      </c>
+      <c r="M17" s="2">
+        <v>314</v>
+      </c>
+      <c r="N17" s="2">
+        <v>11553</v>
+      </c>
+      <c r="O17" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q17" s="2">
+        <v>1</v>
+      </c>
+      <c r="R17" s="2">
+        <v>1617</v>
+      </c>
+      <c r="S17" s="2">
+        <v>41</v>
+      </c>
+      <c r="T17" s="2">
+        <v>2109</v>
+      </c>
+      <c r="U17" s="2">
+        <v>419</v>
+      </c>
+      <c r="V17" s="2">
+        <v>10480</v>
+      </c>
+      <c r="W17" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>2</v>
+      </c>
+      <c r="B18" s="2">
+        <v>899</v>
+      </c>
+      <c r="C18" s="2">
+        <v>800</v>
+      </c>
+      <c r="D18" s="2">
+        <v>2344</v>
+      </c>
+      <c r="E18" s="2">
+        <v>238</v>
+      </c>
+      <c r="F18" s="2">
+        <v>10122</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I18" s="2">
+        <v>2</v>
+      </c>
+      <c r="J18" s="2">
+        <v>1509</v>
+      </c>
+      <c r="K18" s="2">
+        <v>38</v>
+      </c>
+      <c r="L18" s="2">
+        <v>2152</v>
+      </c>
+      <c r="M18" s="2">
+        <v>314</v>
+      </c>
+      <c r="N18" s="2">
+        <v>10527</v>
+      </c>
+      <c r="O18" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q18" s="2">
+        <v>2</v>
+      </c>
+      <c r="R18" s="2">
+        <v>1750</v>
+      </c>
+      <c r="S18" s="2">
+        <v>44</v>
+      </c>
+      <c r="T18" s="2">
+        <v>2272</v>
+      </c>
+      <c r="U18" s="2">
+        <v>394</v>
+      </c>
+      <c r="V18" s="2">
+        <v>11199</v>
+      </c>
+      <c r="W18" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>3</v>
+      </c>
+      <c r="B19" s="2">
+        <v>1006</v>
+      </c>
+      <c r="C19" s="2">
+        <v>652</v>
+      </c>
+      <c r="D19" s="2">
+        <v>2963</v>
+      </c>
+      <c r="E19" s="2">
+        <v>420</v>
+      </c>
+      <c r="F19" s="2">
+        <v>11127</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I19" s="2">
+        <v>3</v>
+      </c>
+      <c r="J19" s="2">
+        <v>1629</v>
+      </c>
+      <c r="K19" s="2">
+        <v>34</v>
+      </c>
+      <c r="L19" s="2">
+        <v>2572</v>
+      </c>
+      <c r="M19" s="2">
+        <v>339</v>
+      </c>
+      <c r="N19" s="2">
+        <v>10769</v>
+      </c>
+      <c r="O19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q19" s="2">
+        <v>3</v>
+      </c>
+      <c r="R19" s="2">
+        <v>1580</v>
+      </c>
+      <c r="S19" s="2">
+        <v>47</v>
+      </c>
+      <c r="T19" s="2">
+        <v>2093</v>
+      </c>
+      <c r="U19" s="2">
+        <v>408</v>
+      </c>
+      <c r="V19" s="2">
+        <v>11085</v>
+      </c>
+      <c r="W19" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>4</v>
+      </c>
+      <c r="B20" s="2">
+        <v>1120</v>
+      </c>
+      <c r="C20" s="2">
+        <v>788</v>
+      </c>
+      <c r="D20" s="2">
+        <v>2928</v>
+      </c>
+      <c r="E20" s="2">
+        <v>322</v>
+      </c>
+      <c r="F20" s="2">
+        <v>11140</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I20" s="2">
+        <v>4</v>
+      </c>
+      <c r="J20" s="2">
+        <v>1780</v>
+      </c>
+      <c r="K20" s="2">
+        <v>33</v>
+      </c>
+      <c r="L20" s="2">
+        <v>2116</v>
+      </c>
+      <c r="M20" s="2">
+        <v>339</v>
+      </c>
+      <c r="N20" s="2">
+        <v>10853</v>
+      </c>
+      <c r="O20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q20" s="2">
+        <v>4</v>
+      </c>
+      <c r="R20" s="2">
+        <v>1779</v>
+      </c>
+      <c r="S20" s="2">
+        <v>49</v>
+      </c>
+      <c r="T20" s="2">
+        <v>2391</v>
+      </c>
+      <c r="U20" s="2">
+        <v>407</v>
+      </c>
+      <c r="V20" s="2">
+        <v>11311</v>
+      </c>
+      <c r="W20" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>5</v>
+      </c>
+      <c r="B21" s="2">
+        <v>898</v>
+      </c>
+      <c r="C21" s="2">
+        <v>652</v>
+      </c>
+      <c r="D21" s="2">
+        <v>2747</v>
+      </c>
+      <c r="E21" s="2">
+        <v>476</v>
+      </c>
+      <c r="F21" s="2">
+        <v>11036</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I21" s="2">
+        <v>5</v>
+      </c>
+      <c r="J21" s="2">
+        <v>1687</v>
+      </c>
+      <c r="K21" s="2">
+        <v>70</v>
+      </c>
+      <c r="L21" s="2">
+        <v>2191</v>
+      </c>
+      <c r="M21" s="2">
+        <v>334</v>
+      </c>
+      <c r="N21" s="2">
+        <v>10779</v>
+      </c>
+      <c r="O21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q21" s="2">
+        <v>5</v>
+      </c>
+      <c r="R21" s="2">
+        <v>1676</v>
+      </c>
+      <c r="S21" s="2">
+        <v>44</v>
+      </c>
+      <c r="T21" s="2">
+        <v>2160</v>
+      </c>
+      <c r="U21" s="2">
+        <v>413</v>
+      </c>
+      <c r="V21" s="2">
+        <v>11586</v>
+      </c>
+      <c r="W21" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>6</v>
+      </c>
+      <c r="B22" s="2">
+        <v>906</v>
+      </c>
+      <c r="C22" s="2">
+        <v>555</v>
+      </c>
+      <c r="D22" s="2">
+        <v>2643</v>
+      </c>
+      <c r="E22" s="2">
+        <v>291</v>
+      </c>
+      <c r="F22" s="2">
+        <v>10395</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I22" s="2">
+        <v>6</v>
+      </c>
+      <c r="J22" s="2">
+        <v>1976</v>
+      </c>
+      <c r="K22" s="2">
+        <v>74</v>
+      </c>
+      <c r="L22" s="2">
+        <v>2414</v>
+      </c>
+      <c r="M22" s="2">
+        <v>349</v>
+      </c>
+      <c r="N22" s="2">
+        <v>11371</v>
+      </c>
+      <c r="O22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q22" s="2">
+        <v>6</v>
+      </c>
+      <c r="R22" s="2">
+        <v>1639</v>
+      </c>
+      <c r="S22" s="2">
+        <v>44</v>
+      </c>
+      <c r="T22" s="2">
+        <v>2325</v>
+      </c>
+      <c r="U22" s="2">
+        <v>387</v>
+      </c>
+      <c r="V22" s="2">
+        <v>11046</v>
+      </c>
+      <c r="W22" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>7</v>
+      </c>
+      <c r="B23" s="2">
+        <v>914</v>
+      </c>
+      <c r="C23" s="2">
+        <v>692</v>
+      </c>
+      <c r="D23" s="2">
+        <v>2675</v>
+      </c>
+      <c r="E23" s="2">
+        <v>258</v>
+      </c>
+      <c r="F23" s="2">
+        <v>11056</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I23" s="2">
+        <v>7</v>
+      </c>
+      <c r="J23" s="2">
+        <v>1479</v>
+      </c>
+      <c r="K23" s="2">
+        <v>44</v>
+      </c>
+      <c r="L23" s="2">
+        <v>2396</v>
+      </c>
+      <c r="M23" s="2">
+        <v>336</v>
+      </c>
+      <c r="N23" s="2">
+        <v>10599</v>
+      </c>
+      <c r="O23" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q23" s="2">
+        <v>7</v>
+      </c>
+      <c r="R23" s="2">
+        <v>1537</v>
+      </c>
+      <c r="S23" s="2">
+        <v>49</v>
+      </c>
+      <c r="T23" s="2">
+        <v>2210</v>
+      </c>
+      <c r="U23" s="2">
+        <v>388</v>
+      </c>
+      <c r="V23" s="2">
+        <v>10689</v>
+      </c>
+      <c r="W23" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>8</v>
+      </c>
+      <c r="B24" s="2">
+        <v>939</v>
+      </c>
+      <c r="C24" s="2">
+        <v>704</v>
+      </c>
+      <c r="D24" s="2">
+        <v>2892</v>
+      </c>
+      <c r="E24" s="2">
+        <v>387</v>
+      </c>
+      <c r="F24" s="2">
+        <v>11223</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I24" s="2">
+        <v>8</v>
+      </c>
+      <c r="J24" s="2">
+        <v>1745</v>
+      </c>
+      <c r="K24" s="2">
+        <v>51</v>
+      </c>
+      <c r="L24" s="2">
+        <v>2325</v>
+      </c>
+      <c r="M24" s="2">
+        <v>315</v>
+      </c>
+      <c r="N24" s="2">
+        <v>10834</v>
+      </c>
+      <c r="O24" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q24" s="2">
+        <v>8</v>
+      </c>
+      <c r="R24" s="2">
+        <v>1614</v>
+      </c>
+      <c r="S24" s="2">
+        <v>38</v>
+      </c>
+      <c r="T24" s="2">
+        <v>2645</v>
+      </c>
+      <c r="U24" s="2">
+        <v>396</v>
+      </c>
+      <c r="V24" s="2">
+        <v>11303</v>
+      </c>
+      <c r="W24" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>9</v>
+      </c>
+      <c r="B25" s="2">
+        <v>978</v>
+      </c>
+      <c r="C25" s="2">
+        <v>701</v>
+      </c>
+      <c r="D25" s="2">
+        <v>2644</v>
+      </c>
+      <c r="E25" s="2">
+        <v>276</v>
+      </c>
+      <c r="F25" s="2">
+        <v>10372</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I25" s="2">
+        <v>9</v>
+      </c>
+      <c r="J25" s="2">
+        <v>1571</v>
+      </c>
+      <c r="K25" s="2">
+        <v>62</v>
+      </c>
+      <c r="L25" s="2">
+        <v>2417</v>
+      </c>
+      <c r="M25" s="2">
+        <v>329</v>
+      </c>
+      <c r="N25" s="2">
+        <v>10473</v>
+      </c>
+      <c r="O25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q25" s="2">
+        <v>9</v>
+      </c>
+      <c r="R25" s="2">
+        <v>1700</v>
+      </c>
+      <c r="S25" s="2">
+        <v>43</v>
+      </c>
+      <c r="T25" s="2">
+        <v>2539</v>
+      </c>
+      <c r="U25" s="2">
+        <v>411</v>
+      </c>
+      <c r="V25" s="2">
+        <v>11186</v>
+      </c>
+      <c r="W25" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>10</v>
+      </c>
+      <c r="B26" s="2">
+        <v>1126</v>
+      </c>
+      <c r="C26" s="2">
+        <v>770</v>
+      </c>
+      <c r="D26" s="2">
+        <v>2354</v>
+      </c>
+      <c r="E26" s="2">
+        <v>270</v>
+      </c>
+      <c r="F26" s="2">
+        <v>10413</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I26" s="2">
+        <v>10</v>
+      </c>
+      <c r="J26" s="2">
+        <v>1585</v>
+      </c>
+      <c r="K26" s="2">
+        <v>48</v>
+      </c>
+      <c r="L26" s="2">
+        <v>2393</v>
+      </c>
+      <c r="M26" s="2">
+        <v>321</v>
+      </c>
+      <c r="N26" s="2">
+        <v>10526</v>
+      </c>
+      <c r="O26" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q26" s="2">
+        <v>10</v>
+      </c>
+      <c r="R26" s="2">
+        <v>1758</v>
+      </c>
+      <c r="S26" s="2">
+        <v>44</v>
+      </c>
+      <c r="T26" s="2">
+        <v>2658</v>
+      </c>
+      <c r="U26" s="2">
+        <v>372</v>
+      </c>
+      <c r="V26" s="2">
+        <v>11588</v>
+      </c>
+      <c r="W26" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="2">
+        <f>AVERAGE(B17:B26)</f>
+        <v>978.5</v>
+      </c>
+      <c r="C27" s="2">
+        <f>AVERAGE(C17:C26)</f>
+        <v>705.5</v>
+      </c>
+      <c r="D27" s="2">
+        <f>AVERAGE(D17:D26)</f>
+        <v>2675.7</v>
+      </c>
+      <c r="E27" s="2">
+        <f>AVERAGE(E17:E26)</f>
+        <v>322.60000000000002</v>
+      </c>
+      <c r="F27" s="2">
+        <f>AVERAGE(F17:F26)</f>
+        <v>10747.1</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J27" s="2">
+        <f>AVERAGE(J17:J26)</f>
+        <v>1686.2</v>
+      </c>
+      <c r="K27" s="2">
+        <f>AVERAGE(K17:K26)</f>
+        <v>49.2</v>
+      </c>
+      <c r="L27" s="2">
+        <f>AVERAGE(L17:L26)</f>
+        <v>2387.4</v>
+      </c>
+      <c r="M27" s="2">
+        <f>AVERAGE(M17:M26)</f>
+        <v>329</v>
+      </c>
+      <c r="N27" s="2">
+        <f>AVERAGE(N17:N26)</f>
+        <v>10828.4</v>
+      </c>
+      <c r="O27" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q27" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="R27" s="2">
+        <f>AVERAGE(R17:R26)</f>
+        <v>1665</v>
+      </c>
+      <c r="S27" s="2">
+        <f>AVERAGE(S17:S26)</f>
+        <v>44.3</v>
+      </c>
+      <c r="T27" s="2">
+        <f>AVERAGE(T17:T26)</f>
+        <v>2340.1999999999998</v>
+      </c>
+      <c r="U27" s="2">
+        <f>AVERAGE(U17:U26)</f>
+        <v>399.5</v>
+      </c>
+      <c r="V27" s="2">
+        <f>AVERAGE(V17:V26)</f>
+        <v>11147.3</v>
+      </c>
+      <c r="W27" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R28" s="2"/>
+      <c r="S28" s="2"/>
+      <c r="T28" s="2"/>
+      <c r="U28" s="2"/>
+      <c r="V28" s="2"/>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="I30" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L30" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="M30" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="N30" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="O30" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="I31" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K31" s="2">
+        <v>609.70000000000005</v>
+      </c>
+      <c r="L31" s="2">
+        <v>1454.3</v>
+      </c>
+      <c r="M31" s="2">
+        <v>306.89999999999998</v>
+      </c>
+      <c r="N31" s="2">
+        <v>98.1</v>
+      </c>
+      <c r="O31" s="2">
+        <v>6603.3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="I32" s="3"/>
+      <c r="J32" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K32" s="2">
+        <v>978.5</v>
+      </c>
+      <c r="L32" s="2">
+        <v>2675.7</v>
+      </c>
+      <c r="M32" s="2">
+        <v>322.60000000000002</v>
+      </c>
+      <c r="N32" s="2">
+        <v>705.5</v>
+      </c>
+      <c r="O32" s="2">
+        <v>10747.1</v>
+      </c>
+    </row>
+    <row r="33" spans="9:15" x14ac:dyDescent="0.25">
+      <c r="I33" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K33" s="2">
+        <v>922</v>
+      </c>
+      <c r="L33" s="2">
+        <v>1125.4000000000001</v>
+      </c>
+      <c r="M33" s="2">
+        <v>330.1</v>
+      </c>
+      <c r="N33" s="2">
+        <v>36.6</v>
+      </c>
+      <c r="O33" s="2">
+        <v>6120.9</v>
+      </c>
+    </row>
+    <row r="34" spans="9:15" x14ac:dyDescent="0.25">
+      <c r="I34" s="3"/>
+      <c r="J34" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K34" s="2">
+        <v>1686.2</v>
+      </c>
+      <c r="L34" s="2">
+        <v>2387.4</v>
+      </c>
+      <c r="M34" s="2">
+        <v>329</v>
+      </c>
+      <c r="N34" s="2">
+        <v>49.2</v>
+      </c>
+      <c r="O34" s="2">
+        <v>10828.4</v>
+      </c>
+    </row>
+    <row r="35" spans="9:15" x14ac:dyDescent="0.25">
+      <c r="I35" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K35" s="2">
+        <v>823.4</v>
+      </c>
+      <c r="L35" s="2">
+        <v>1122.0999999999999</v>
+      </c>
+      <c r="M35" s="2">
+        <v>379</v>
+      </c>
+      <c r="N35" s="2">
+        <v>20.9</v>
+      </c>
+      <c r="O35" s="2">
+        <v>6092.3</v>
+      </c>
+    </row>
+    <row r="36" spans="9:15" x14ac:dyDescent="0.25">
+      <c r="I36" s="3"/>
+      <c r="J36" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K36" s="2">
+        <v>1665</v>
+      </c>
+      <c r="L36" s="2">
+        <v>2340.1999999999998</v>
+      </c>
+      <c r="M36" s="2">
+        <v>399.5</v>
+      </c>
+      <c r="N36" s="2">
+        <v>44.3</v>
+      </c>
+      <c r="O36" s="2">
+        <v>11147.3</v>
+      </c>
+    </row>
+    <row r="37" spans="9:15" x14ac:dyDescent="0.25">
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+      <c r="N37" s="2"/>
+      <c r="O37" s="2"/>
+    </row>
+    <row r="38" spans="9:15" x14ac:dyDescent="0.25">
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="2"/>
+      <c r="M38" s="2"/>
+      <c r="N38" s="2"/>
+      <c r="O38" s="2"/>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="I31:I32"/>
+    <mergeCell ref="I33:I34"/>
+    <mergeCell ref="I35:I36"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>